<commit_message>
database api end-to-end automation
</commit_message>
<xml_diff>
--- a/test_data/ReadData.xlsx
+++ b/test_data/ReadData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buraksimsek/IdeaProjects/backend_automation_b6/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C8AF9B-7364-3F4C-8AC4-54B02C7D45AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFDF3DA-A1D9-FF40-AB71-2AA69F728FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10200" yWindow="4360" windowWidth="28040" windowHeight="17440" xr2:uid="{D27C0761-34E1-F542-B6FE-3C8CFA8ECAF7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Active</t>
+  </si>
+  <si>
+    <t>ops</t>
   </si>
 </sst>
 </file>
@@ -414,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3E4B42-D171-8745-827A-7D9DFE8E5E23}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -467,6 +470,20 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>